<commit_message>
add new words in excel
</commit_message>
<xml_diff>
--- a/daily_new_words.xlsx
+++ b/daily_new_words.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangyifan/Desktop/WordTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A765D73B-2494-6648-A14B-DAE6D6159210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F625058-1452-234B-8658-0DCC368DEFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{B5BDFF85-3964-334A-A517-303E07D821B6}"/>
+    <workbookView xWindow="17680" yWindow="880" windowWidth="10640" windowHeight="16540" activeTab="1" xr2:uid="{B5BDFF85-3964-334A-A517-303E07D821B6}"/>
   </bookViews>
   <sheets>
     <sheet name="2025-08-10" sheetId="1" r:id="rId1"/>
+    <sheet name="2025-08-11" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
   <si>
     <t>唯利是图的</t>
   </si>
@@ -225,6 +226,156 @@
   </si>
   <si>
     <t>resemble</t>
+  </si>
+  <si>
+    <t>有血有肉的</t>
+  </si>
+  <si>
+    <t>flesh-and-blood</t>
+  </si>
+  <si>
+    <t>撤回</t>
+  </si>
+  <si>
+    <t>retraction</t>
+  </si>
+  <si>
+    <t>揭露丑闻</t>
+  </si>
+  <si>
+    <t>muckraking</t>
+  </si>
+  <si>
+    <t>笨重的</t>
+  </si>
+  <si>
+    <t>bulky</t>
+  </si>
+  <si>
+    <t>预言</t>
+  </si>
+  <si>
+    <t>divine</t>
+  </si>
+  <si>
+    <t>追踪</t>
+  </si>
+  <si>
+    <t>trace</t>
+  </si>
+  <si>
+    <t>挖掘</t>
+  </si>
+  <si>
+    <t>excavations</t>
+  </si>
+  <si>
+    <t>吝啬</t>
+  </si>
+  <si>
+    <t>parsimony</t>
+  </si>
+  <si>
+    <t>投机主义</t>
+  </si>
+  <si>
+    <t>opportunism</t>
+  </si>
+  <si>
+    <t>miserliness</t>
+  </si>
+  <si>
+    <t>讨厌的东西</t>
+  </si>
+  <si>
+    <t>nuisance</t>
+  </si>
+  <si>
+    <t>意外收获</t>
+  </si>
+  <si>
+    <t>windfall</t>
+  </si>
+  <si>
+    <t>引起</t>
+  </si>
+  <si>
+    <t>invoke</t>
+  </si>
+  <si>
+    <t>同意</t>
+  </si>
+  <si>
+    <t>concur</t>
+  </si>
+  <si>
+    <t>井然有序的</t>
+  </si>
+  <si>
+    <t>methodical</t>
+  </si>
+  <si>
+    <t>尽管</t>
+  </si>
+  <si>
+    <t>that said</t>
+  </si>
+  <si>
+    <t>开玩笑</t>
+  </si>
+  <si>
+    <t>jest</t>
+  </si>
+  <si>
+    <t>开放性的</t>
+  </si>
+  <si>
+    <t>expansive</t>
+  </si>
+  <si>
+    <t>细小的</t>
+  </si>
+  <si>
+    <t>fine</t>
+  </si>
+  <si>
+    <t>尴尬</t>
+  </si>
+  <si>
+    <t>discomfiture</t>
+  </si>
+  <si>
+    <t>presumptuousness</t>
+  </si>
+  <si>
+    <t>自以为是</t>
+  </si>
+  <si>
+    <t>细心</t>
+  </si>
+  <si>
+    <t>circumspection</t>
+  </si>
+  <si>
+    <t>颁布</t>
+  </si>
+  <si>
+    <t>promulgated</t>
+  </si>
+  <si>
+    <t>误解</t>
+  </si>
+  <si>
+    <t>misconstrued</t>
+  </si>
+  <si>
+    <t>壁画</t>
+  </si>
+  <si>
+    <t>mural</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -598,7 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18972A3-7D54-E74D-949B-5202DFDA662F}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="167" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="167" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -863,4 +1014,224 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72295E5-1C72-2A48-98AD-C40B2939DB8F}">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>